<commit_message>
Edits based on Ji's comments.
</commit_message>
<xml_diff>
--- a/figs_src/imp-whiskers.xlsx
+++ b/figs_src/imp-whiskers.xlsx
@@ -733,11 +733,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="141059200"/>
-        <c:axId val="141060736"/>
+        <c:axId val="152389504"/>
+        <c:axId val="152391040"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="141059200"/>
+        <c:axId val="152389504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -754,7 +754,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="141060736"/>
+        <c:crossAx val="152391040"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -762,7 +762,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="141060736"/>
+        <c:axId val="152391040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -790,7 +790,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="141059200"/>
+        <c:crossAx val="152389504"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1295,11 +1295,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="141095680"/>
-        <c:axId val="141097216"/>
+        <c:axId val="152434176"/>
+        <c:axId val="152435712"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="141095680"/>
+        <c:axId val="152434176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1316,7 +1316,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="141097216"/>
+        <c:crossAx val="152435712"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1324,7 +1324,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="141097216"/>
+        <c:axId val="152435712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1352,7 +1352,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="141095680"/>
+        <c:crossAx val="152434176"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2076,11 +2076,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="141158272"/>
-        <c:axId val="141159808"/>
+        <c:axId val="152480384"/>
+        <c:axId val="152494464"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="141158272"/>
+        <c:axId val="152480384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2097,7 +2097,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="141159808"/>
+        <c:crossAx val="152494464"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2105,7 +2105,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="141159808"/>
+        <c:axId val="152494464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2133,7 +2133,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="141158272"/>
+        <c:crossAx val="152480384"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2148,7 +2148,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2989,11 +2988,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="100"/>
-        <c:axId val="92279168"/>
-        <c:axId val="92281088"/>
+        <c:axId val="152662400"/>
+        <c:axId val="152663936"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="92279168"/>
+        <c:axId val="152662400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3002,7 +3001,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92281088"/>
+        <c:crossAx val="152663936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3010,7 +3009,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="92281088"/>
+        <c:axId val="152663936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.1"/>
@@ -3018,11 +3017,30 @@
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Error</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="0.0%" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92279168"/>
+        <c:crossAx val="152662400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3639,11 +3657,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="141696000"/>
-        <c:axId val="141697792"/>
+        <c:axId val="152769664"/>
+        <c:axId val="152771200"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="141696000"/>
+        <c:axId val="152769664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3660,7 +3678,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="141697792"/>
+        <c:crossAx val="152771200"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3668,7 +3686,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="141697792"/>
+        <c:axId val="152771200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3696,7 +3714,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="141696000"/>
+        <c:crossAx val="152769664"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3741,7 +3759,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="156" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="160" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="159" orientation="portrait" r:id="rId1"/>
@@ -3848,7 +3866,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="6276731" cy="2173654"/>
+    <xdr:ext cx="6125766" cy="2024063"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>

</xml_diff>